<commit_message>
correction: add Rwanda to ECCAS
</commit_message>
<xml_diff>
--- a/raw_data/UNICEF_SP/UNICEF Programme Countries and Territories.xlsx
+++ b/raw_data/UNICEF_SP/UNICEF Programme Countries and Territories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef.sharepoint.com/teams/DAPM-ChildMortality/Shared Documents/UN IGME data/update country.info.CME/Regional Groupings/2024/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef.sharepoint.com/teams/DAPM-ChildMortality/Shared Documents/UN IGME data/update country.info.CME/Country-and-Region-Metadata/raw_data/UNICEF_SP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{B7DC84C0-E05A-4820-85C7-3CB92466A068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16128CA8-827B-4C94-BF08-8F5C99DDEA1A}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{B7DC84C0-E05A-4820-85C7-3CB92466A068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63E34998-E773-4949-8319-0B96D40DC5F8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="705" windowWidth="24165" windowHeight="15825" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source Data" sheetId="3" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6157,7 +6157,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B621DB84-86AF-443A-9C10-F2C64C0D3F73}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B621DB84-86AF-443A-9C10-F2C64C0D3F73}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G6:H65" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="19">
     <pivotField axis="axisRow" showAll="0">
@@ -6670,7 +6670,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B716518-FB00-465B-A5A0-713261B85A8A}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0B716518-FB00-465B-A5A0-713261B85A8A}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M6:N53" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="19">
     <pivotField showAll="0"/>
@@ -7030,7 +7030,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9ECED581-2CC3-44F8-BD46-6F158EB07780}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9ECED581-2CC3-44F8-BD46-6F158EB07780}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D6:E140" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="19">
     <pivotField axis="axisRow" showAll="0">
@@ -7666,7 +7666,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1D3D1D2-5EAE-405E-8599-B9B3C5D30CE0}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Region">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E1D3D1D2-5EAE-405E-8599-B9B3C5D30CE0}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Region">
   <location ref="A6:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="19">
     <pivotField axis="axisRow" showAll="0">
@@ -7924,7 +7924,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4540031-F45F-48D9-8695-B00253242FD6}" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4540031-F45F-48D9-8695-B00253242FD6}" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J6:K13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="19">
     <pivotField axis="axisRow" showAll="0">
@@ -8177,13 +8177,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1E30B81C-A21E-4E39-A2F2-4D9F002239DF}" name="Table13" displayName="Table13" ref="A1:S159" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
-  <autoFilter ref="A1:S159" xr:uid="{1E30B81C-A21E-4E39-A2F2-4D9F002239DF}">
-    <filterColumn colId="16">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:S159" xr:uid="{1E30B81C-A21E-4E39-A2F2-4D9F002239DF}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{D93C4708-22CF-4590-8683-C4C3BBAA81FE}" name="Region" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{BC140D95-379E-4BF4-A877-7605F05D215A}" name="BA Code" dataDxfId="19"/>
@@ -8513,10 +8507,10 @@
   <dimension ref="A1:S159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R35" sqref="R35"/>
+      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8647,7 +8641,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -8683,7 +8677,7 @@
       </c>
       <c r="Q3" s="8"/>
     </row>
-    <row r="4" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -8767,7 +8761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -8806,7 +8800,7 @@
       </c>
       <c r="Q6" s="8"/>
     </row>
-    <row r="7" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -8845,7 +8839,7 @@
       </c>
       <c r="Q7" s="8"/>
     </row>
-    <row r="8" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -8918,7 +8912,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -8954,7 +8948,7 @@
       </c>
       <c r="Q10" s="8"/>
     </row>
-    <row r="11" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -9036,7 +9030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -9072,7 +9066,7 @@
       </c>
       <c r="Q13" s="8"/>
     </row>
-    <row r="14" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -9152,7 +9146,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -9192,7 +9186,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -9229,7 +9223,7 @@
       <c r="Q17" s="8"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -9267,7 +9261,7 @@
       </c>
       <c r="Q18" s="8"/>
     </row>
-    <row r="19" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -9308,7 +9302,7 @@
       </c>
       <c r="Q19" s="8"/>
     </row>
-    <row r="20" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -9344,7 +9338,7 @@
       </c>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -9475,7 +9469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -9516,7 +9510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>72</v>
       </c>
@@ -9550,7 +9544,7 @@
       <c r="Q25" s="8"/>
       <c r="R25"/>
     </row>
-    <row r="26" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>103</v>
       </c>
@@ -9680,7 +9674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -9715,7 +9709,7 @@
       </c>
       <c r="Q29" s="8"/>
     </row>
-    <row r="30" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>103</v>
       </c>
@@ -9748,7 +9742,7 @@
       </c>
       <c r="Q30" s="8"/>
     </row>
-    <row r="31" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>38</v>
       </c>
@@ -9786,7 +9780,7 @@
       </c>
       <c r="Q31" s="8"/>
     </row>
-    <row r="32" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -9822,7 +9816,7 @@
       </c>
       <c r="Q32" s="8"/>
     </row>
-    <row r="33" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>72</v>
       </c>
@@ -9861,7 +9855,7 @@
       <c r="Q33" s="8"/>
       <c r="R33"/>
     </row>
-    <row r="34" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -9940,7 +9934,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>72</v>
       </c>
@@ -9980,7 +9974,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>25</v>
       </c>
@@ -10018,7 +10012,7 @@
       </c>
       <c r="Q37" s="8"/>
     </row>
-    <row r="38" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -10102,7 +10096,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>30</v>
       </c>
@@ -10143,7 +10137,7 @@
       </c>
       <c r="Q40" s="8"/>
     </row>
-    <row r="41" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -10182,7 +10176,7 @@
       </c>
       <c r="Q41" s="8"/>
     </row>
-    <row r="42" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -10220,7 +10214,7 @@
       </c>
       <c r="Q42" s="8"/>
     </row>
-    <row r="43" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>103</v>
       </c>
@@ -10253,7 +10247,7 @@
       </c>
       <c r="Q43" s="8"/>
     </row>
-    <row r="44" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -10374,7 +10368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -10456,7 +10450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>34</v>
       </c>
@@ -10540,7 +10534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -10576,7 +10570,7 @@
       </c>
       <c r="Q51" s="8"/>
     </row>
-    <row r="52" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -10610,7 +10604,7 @@
       <c r="Q52" s="8"/>
       <c r="R52"/>
     </row>
-    <row r="53" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -10647,7 +10641,7 @@
       <c r="Q53" s="8"/>
       <c r="R53"/>
     </row>
-    <row r="54" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -10685,7 +10679,7 @@
       </c>
       <c r="Q54" s="8"/>
     </row>
-    <row r="55" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>72</v>
       </c>
@@ -10725,7 +10719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>25</v>
       </c>
@@ -10763,7 +10757,7 @@
       </c>
       <c r="Q56" s="8"/>
     </row>
-    <row r="57" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -10802,7 +10796,7 @@
       </c>
       <c r="Q57" s="8"/>
     </row>
-    <row r="58" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -10886,7 +10880,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -10923,7 +10917,7 @@
       <c r="Q60" s="8"/>
       <c r="R60"/>
     </row>
-    <row r="61" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -11095,7 +11089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>103</v>
       </c>
@@ -11226,7 +11220,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -11299,7 +11293,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>25</v>
       </c>
@@ -11380,7 +11374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>103</v>
       </c>
@@ -11419,7 +11413,7 @@
       </c>
       <c r="Q72" s="8"/>
     </row>
-    <row r="73" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>25</v>
       </c>
@@ -11455,7 +11449,7 @@
       </c>
       <c r="Q73" s="8"/>
     </row>
-    <row r="74" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>30</v>
       </c>
@@ -11491,7 +11485,7 @@
       </c>
       <c r="Q74" s="8"/>
     </row>
-    <row r="75" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>103</v>
       </c>
@@ -11577,7 +11571,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -11613,7 +11607,7 @@
       </c>
       <c r="Q77" s="8"/>
     </row>
-    <row r="78" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>72</v>
       </c>
@@ -11789,7 +11783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>103</v>
       </c>
@@ -11825,7 +11819,7 @@
       </c>
       <c r="Q82" s="8"/>
     </row>
-    <row r="83" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -11910,7 +11904,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>103</v>
       </c>
@@ -12037,7 +12031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>103</v>
       </c>
@@ -12121,7 +12115,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>103</v>
       </c>
@@ -12157,7 +12151,7 @@
       </c>
       <c r="Q90" s="8"/>
     </row>
-    <row r="91" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>38</v>
       </c>
@@ -12196,7 +12190,7 @@
       </c>
       <c r="Q91" s="8"/>
     </row>
-    <row r="92" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>30</v>
       </c>
@@ -12274,7 +12268,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>34</v>
       </c>
@@ -12310,7 +12304,7 @@
       </c>
       <c r="Q94" s="8"/>
     </row>
-    <row r="95" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>103</v>
       </c>
@@ -12349,7 +12343,7 @@
       </c>
       <c r="Q95" s="8"/>
     </row>
-    <row r="96" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -12391,7 +12385,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>38</v>
       </c>
@@ -12523,7 +12517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>103</v>
       </c>
@@ -12562,7 +12556,7 @@
       </c>
       <c r="Q100" s="8"/>
     </row>
-    <row r="101" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>25</v>
       </c>
@@ -12598,7 +12592,7 @@
       </c>
       <c r="Q101" s="8"/>
     </row>
-    <row r="102" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>30</v>
       </c>
@@ -12685,7 +12679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -12811,7 +12805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>103</v>
       </c>
@@ -12850,7 +12844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>38</v>
       </c>
@@ -12886,7 +12880,7 @@
       </c>
       <c r="Q108" s="8"/>
     </row>
-    <row r="109" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>38</v>
       </c>
@@ -12924,7 +12918,7 @@
       </c>
       <c r="Q109" s="8"/>
     </row>
-    <row r="110" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>103</v>
       </c>
@@ -12965,7 +12959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -13001,7 +12995,7 @@
       </c>
       <c r="Q111" s="8"/>
     </row>
-    <row r="112" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>25</v>
       </c>
@@ -13087,7 +13081,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>25</v>
       </c>
@@ -13123,7 +13117,7 @@
       </c>
       <c r="Q114" s="8"/>
     </row>
-    <row r="115" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>25</v>
       </c>
@@ -13254,7 +13248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>34</v>
       </c>
@@ -13293,7 +13287,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>38</v>
       </c>
@@ -13332,7 +13326,7 @@
       </c>
       <c r="Q119" s="8"/>
     </row>
-    <row r="120" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>103</v>
       </c>
@@ -13371,7 +13365,7 @@
       </c>
       <c r="Q120" s="8"/>
     </row>
-    <row r="121" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>72</v>
       </c>
@@ -13404,7 +13398,7 @@
       </c>
       <c r="Q121" s="8"/>
     </row>
-    <row r="122" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>30</v>
       </c>
@@ -13437,7 +13431,7 @@
       </c>
       <c r="Q122" s="8"/>
     </row>
-    <row r="123" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>72</v>
       </c>
@@ -13476,7 +13470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>25</v>
       </c>
@@ -13517,7 +13511,7 @@
       </c>
       <c r="Q124" s="8"/>
     </row>
-    <row r="125" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>72</v>
       </c>
@@ -13556,7 +13550,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>103</v>
       </c>
@@ -13643,7 +13637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>34</v>
       </c>
@@ -13770,7 +13764,7 @@
       </c>
       <c r="R130"/>
     </row>
-    <row r="131" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>38</v>
       </c>
@@ -13809,7 +13803,7 @@
       </c>
       <c r="Q131" s="8"/>
     </row>
-    <row r="132" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>38</v>
       </c>
@@ -13896,7 +13890,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>38</v>
       </c>
@@ -13983,7 +13977,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>25</v>
       </c>
@@ -14024,7 +14018,7 @@
       </c>
       <c r="Q136" s="8"/>
     </row>
-    <row r="137" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>103</v>
       </c>
@@ -14060,7 +14054,7 @@
       </c>
       <c r="Q137" s="8"/>
     </row>
-    <row r="138" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>103</v>
       </c>
@@ -14096,7 +14090,7 @@
       </c>
       <c r="Q138" s="8"/>
     </row>
-    <row r="139" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>72</v>
       </c>
@@ -14135,7 +14129,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>103</v>
       </c>
@@ -14174,7 +14168,7 @@
       </c>
       <c r="Q140" s="8"/>
     </row>
-    <row r="141" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>103</v>
       </c>
@@ -14213,7 +14207,7 @@
       </c>
       <c r="Q141" s="8"/>
     </row>
-    <row r="142" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>38</v>
       </c>
@@ -14254,7 +14248,7 @@
       </c>
       <c r="Q142" s="8"/>
     </row>
-    <row r="143" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>30</v>
       </c>
@@ -14337,7 +14331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="145" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>25</v>
       </c>
@@ -14378,7 +14372,7 @@
       </c>
       <c r="Q145" s="8"/>
     </row>
-    <row r="146" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>38</v>
       </c>
@@ -14417,7 +14411,7 @@
       </c>
       <c r="Q146" s="8"/>
     </row>
-    <row r="147" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>103</v>
       </c>
@@ -14546,7 +14540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>34</v>
       </c>
@@ -14585,7 +14579,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>38</v>
       </c>
@@ -14620,7 +14614,7 @@
       </c>
       <c r="Q151" s="8"/>
     </row>
-    <row r="152" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>30</v>
       </c>
@@ -14656,7 +14650,7 @@
       </c>
       <c r="Q152" s="8"/>
     </row>
-    <row r="153" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>103</v>
       </c>
@@ -14743,7 +14737,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>103</v>
       </c>
@@ -14779,7 +14773,7 @@
       </c>
       <c r="Q155" s="8"/>
     </row>
-    <row r="156" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>38</v>
       </c>
@@ -14866,7 +14860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:19" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>34</v>
       </c>
@@ -19710,6 +19704,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocId xmlns="37893236-cb76-4d6f-8a18-4c624154e39c">RFF2MQFYXHK7-870072624-105835</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="37893236-cb76-4d6f-8a18-4c624154e39c">
+      <Url>https://unicef.sharepoint.com/teams/DAPM-ChildMortality/_layouts/15/DocIdRedir.aspx?ID=RFF2MQFYXHK7-870072624-105835</Url>
+      <Description>RFF2MQFYXHK7-870072624-105835</Description>
+    </_dlc_DocIdUrl>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8563a7a-d9fa-431f-b50c-34632ce7e22e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -19757,31 +19776,6 @@
     <Filter/>
   </Receiver>
 </spe:Receivers>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocId xmlns="37893236-cb76-4d6f-8a18-4c624154e39c">RFF2MQFYXHK7-870072624-105835</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="37893236-cb76-4d6f-8a18-4c624154e39c">
-      <Url>https://unicef.sharepoint.com/teams/DAPM-ChildMortality/_layouts/15/DocIdRedir.aspx?ID=RFF2MQFYXHK7-870072624-105835</Url>
-      <Description>RFF2MQFYXHK7-870072624-105835</Description>
-    </_dlc_DocIdUrl>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8563a7a-d9fa-431f-b50c-34632ce7e22e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20064,9 +20058,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DACE9A66-F0B1-41C6-AEBA-CB8FF210E1AD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72875380-4ED0-4C9C-BC51-9F7619DFA317}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20088,9 +20082,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72875380-4ED0-4C9C-BC51-9F7619DFA317}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DACE9A66-F0B1-41C6-AEBA-CB8FF210E1AD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>